<commit_message>
Resuelto conflicto en db.sqlite y conservada la versión local
</commit_message>
<xml_diff>
--- a/backend/data/inventario.xlsx
+++ b/backend/data/inventario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sara\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B2344E-10DD-4235-B95F-E6314EF92569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97BE358A-672E-4A2B-AD6E-E5FDEFC714A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +602,7 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>150</v>

</xml_diff>